<commit_message>
Replacing Studio Groom with new Groom.
</commit_message>
<xml_diff>
--- a/Examples/Studio/Ellipsoid/ellipsoid.xlsx
+++ b/Examples/Studio/Ellipsoid/ellipsoid.xlsx
@@ -13,17 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="groom" sheetId="29" r:id="rId2"/>
-    <sheet name="optimize" sheetId="30" r:id="rId3"/>
-    <sheet name="analysis" sheetId="31" r:id="rId4"/>
-    <sheet name="studio" sheetId="32" r:id="rId5"/>
+    <sheet name="groom" sheetId="33" r:id="rId2"/>
+    <sheet name="optimize" sheetId="34" r:id="rId3"/>
+    <sheet name="analysis" sheetId="35" r:id="rId4"/>
+    <sheet name="studio" sheetId="36" r:id="rId5"/>
+    <sheet name="project" sheetId="37" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -185,6 +186,49 @@
   </si>
   <si>
     <t>Original</t>
+  </si>
+  <si>
+    <t>initial_relative_weighting</t>
+  </si>
+  <si>
+    <t>multiscale</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>multiscale_particles</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>normals_strength</t>
+  </si>
+  <si>
+    <t>procrustes</t>
+  </si>
+  <si>
+    <t>procrustes_scaling</t>
+  </si>
+  <si>
+    <t>use_normals</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE HTML PUBLIC "-//W3C//DTD HTML 4.0//EN" "http://www.w3.org/TR/REC-html40/strict.dtd"&gt;
+&lt;html&gt;&lt;head&gt;&lt;meta name="qrichtext" content="1" /&gt;&lt;style type="text/css"&gt;
+p, li { white-space: pre-wrap; }
+&lt;/style&gt;&lt;/head&gt;&lt;body style=" font-family:'.AppleSystemUIFont'; font-size:13pt; font-weight:400; font-style:normal;"&gt;
+&lt;p style="-qt-paragraph-type:empty; margin-top:0px; margin-bottom:0px; margin-left:0px; margin-right:0px; -qt-block-indent:0; text-indent:0px;"&gt;&lt;br /&gt;&lt;/p&gt;&lt;/body&gt;&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -565,7 +609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -662,9 +706,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B15"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
@@ -685,57 +729,113 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B14" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -776,9 +876,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
@@ -799,26 +899,59 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switch and fix parameters
</commit_message>
<xml_diff>
--- a/Examples/Studio/Ellipsoid/ellipsoid.xlsx
+++ b/Examples/Studio/Ellipsoid/ellipsoid.xlsx
@@ -13,18 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="groom" sheetId="33" r:id="rId2"/>
-    <sheet name="optimize" sheetId="34" r:id="rId3"/>
-    <sheet name="analysis" sheetId="35" r:id="rId4"/>
-    <sheet name="studio" sheetId="36" r:id="rId5"/>
-    <sheet name="project" sheetId="37" r:id="rId6"/>
+    <sheet name="groom" sheetId="83" r:id="rId2"/>
+    <sheet name="optimize" sheetId="84" r:id="rId3"/>
+    <sheet name="analysis" sheetId="85" r:id="rId4"/>
+    <sheet name="studio" sheetId="86" r:id="rId5"/>
+    <sheet name="project" sheetId="87" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -229,6 +229,54 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>antilias</t>
+  </si>
+  <si>
+    <t>groomed_file</t>
+  </si>
+  <si>
+    <t>ellipsoid_1_DT.nrrd</t>
+  </si>
+  <si>
+    <t>transform_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000</t>
+  </si>
+  <si>
+    <t>ellipsoid_2_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_3_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_4_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_5_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_6_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_7_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_8_DT.nrrd</t>
+  </si>
+  <si>
+    <t>ellipsoid_9_DT.nrrd</t>
+  </si>
+  <si>
+    <t>feature_map</t>
+  </si>
+  <si>
+    <t>-none-</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -543,7 +591,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
@@ -554,54 +602,114 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -609,9 +717,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
@@ -640,31 +748,31 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -672,7 +780,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -680,7 +788,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -688,7 +796,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -696,9 +804,17 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -706,7 +822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -835,7 +951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -876,9 +992,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
@@ -899,33 +1015,41 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -933,7 +1057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Restore ellipsoid to pre-run state
</commit_message>
<xml_diff>
--- a/Examples/Studio/Ellipsoid/ellipsoid.xlsx
+++ b/Examples/Studio/Ellipsoid/ellipsoid.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Examples/Studio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Examples/Studio/Ellipsoid/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDABC9A9-189B-3D47-A2EF-EC5CDF78BE7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -177,12 +178,6 @@
   </si>
   <si>
     <t>groom</t>
-  </si>
-  <si>
-    <t>Groomed</t>
-  </si>
-  <si>
-    <t>data</t>
   </si>
   <si>
     <t>Original</t>
@@ -234,55 +229,16 @@
     <t>antilias</t>
   </si>
   <si>
-    <t>groomed_file</t>
-  </si>
-  <si>
-    <t>ellipsoid_1_DT.nrrd</t>
-  </si>
-  <si>
-    <t>transform_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000</t>
-  </si>
-  <si>
-    <t>ellipsoid_2_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_3_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_4_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_5_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_6_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_7_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_8_DT.nrrd</t>
-  </si>
-  <si>
-    <t>ellipsoid_9_DT.nrrd</t>
-  </si>
-  <si>
     <t>feature_map</t>
   </si>
   <si>
     <t>-none-</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -323,6 +279,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -590,11 +549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,114 +561,54 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -717,12 +616,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B12"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -730,7 +632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -738,7 +640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -746,15 +648,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -762,7 +664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -770,7 +672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -778,7 +680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -786,7 +688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -794,7 +696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -802,7 +704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -810,7 +712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -819,15 +721,19 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B15"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -835,7 +741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -843,15 +749,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -859,31 +765,31 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>57</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -891,7 +797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -899,15 +805,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -915,15 +821,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -931,7 +837,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -939,24 +845,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -964,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -972,7 +882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -980,7 +890,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -989,15 +899,21 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B7"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1005,7 +921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1013,23 +929,23 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1037,7 +953,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1045,7 +961,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -1054,15 +970,19 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1070,14 +990,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Grooming for image domain now writes meshes.
</commit_message>
<xml_diff>
--- a/Examples/Studio/Ellipsoid/ellipsoid.xlsx
+++ b/Examples/Studio/Ellipsoid/ellipsoid.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amorris/sci/shapeworks/code/Examples/Studio/Ellipsoid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDABC9A9-189B-3D47-A2EF-EC5CDF78BE7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>segmentation_file</t>
   </si>
@@ -234,11 +233,74 @@
   <si>
     <t>-none-</t>
   </si>
+  <si>
+    <t>groomed_file</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_1_DT.nrrd</t>
+  </si>
+  <si>
+    <t>alignment_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -39.999849 -49.999811 -49.999811</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_2_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -42.499850 -50.000000 -50.000000</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_3_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -44.999848 -49.999831 -49.999831</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_4_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -47.499850 -50.000000 -50.000000</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_5_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -49.999851 -49.999851 -49.999851</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_6_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -52.499850 -50.000000 -50.000000</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_7_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -54.999699 -49.999862 -49.999862</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_8_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -57.499850 -50.000000 -50.000000</t>
+  </si>
+  <si>
+    <t>./groomed/ellipsoid_9_DT.nrrd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.000000 0.000000 0.000000 0.000000 1.000000 0.000000 0.000000 0.000000 1.000000 -59.999700 -49.999873 -49.999873</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -279,9 +341,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -549,10 +608,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -561,54 +620,114 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -617,12 +736,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -726,12 +845,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -859,12 +978,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -904,14 +1023,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -975,12 +1094,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -995,7 +1114,7 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>